<commit_message>
Update contents with Camille remark's
</commit_message>
<xml_diff>
--- a/exercises/data/phenotype.xlsx
+++ b/exercises/data/phenotype.xlsx
@@ -525,7 +525,7 @@
   <dimension ref="A1:BA89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="118" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,7 +624,7 @@
         <v>0.92999999999999994</v>
       </c>
       <c r="G2" s="11">
-        <v>0.66999999999999993</v>
+        <v>1.67</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -656,7 +656,7 @@
         <v>0.95300000000000007</v>
       </c>
       <c r="G3" s="11">
-        <v>0.72</v>
+        <v>1.72</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -688,7 +688,7 @@
         <v>1.04</v>
       </c>
       <c r="G4" s="11">
-        <v>1.002</v>
+        <v>2.0019999999999998</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -720,7 +720,7 @@
         <v>0.70599999999999996</v>
       </c>
       <c r="G5" s="11">
-        <v>0.43399999999999994</v>
+        <v>1.4339999999999999</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -752,7 +752,7 @@
         <v>2.31</v>
       </c>
       <c r="G6" s="11">
-        <v>2.7669999999999999</v>
+        <v>3.7669999999999999</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -784,7 +784,7 @@
         <v>2.2199999999999998</v>
       </c>
       <c r="G7" s="11">
-        <v>3.6619999999999999</v>
+        <v>4.6619999999999999</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -816,7 +816,7 @@
         <v>2.4709999999999996</v>
       </c>
       <c r="G8" s="11">
-        <v>4.0789999999999997</v>
+        <v>5.0789999999999997</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -880,7 +880,7 @@
         <v>1.2049999999999998</v>
       </c>
       <c r="G10" s="11">
-        <v>1.0939999999999999</v>
+        <v>2.0939999999999999</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -912,7 +912,7 @@
         <v>1.8779999999999999</v>
       </c>
       <c r="G11" s="11">
-        <v>2.0589999999999997</v>
+        <v>3.0589999999999997</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -944,7 +944,7 @@
         <v>1.6479999999999999</v>
       </c>
       <c r="G12" s="11">
-        <v>1.8660000000000001</v>
+        <v>2.8660000000000001</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -976,7 +976,7 @@
         <v>1.9689999999999999</v>
       </c>
       <c r="G13" s="11">
-        <v>2.4699999999999998</v>
+        <v>3.4699999999999998</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1008,7 +1008,7 @@
         <v>2.9499999999999997</v>
       </c>
       <c r="G14" s="11">
-        <v>4.7679999999999998</v>
+        <v>5.7679999999999998</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -1040,7 +1040,7 @@
         <v>3.9119999999999995</v>
       </c>
       <c r="G15" s="11">
-        <v>6.149</v>
+        <v>7.149</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1072,7 +1072,7 @@
         <v>3.1749999999999998</v>
       </c>
       <c r="G16" s="11">
-        <v>5.1109999999999998</v>
+        <v>6.1109999999999998</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -1104,7 +1104,7 @@
         <v>2.7199999999999998</v>
       </c>
       <c r="G17" s="11">
-        <v>4.0299999999999994</v>
+        <v>5.0299999999999994</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -1136,7 +1136,7 @@
         <v>5.01</v>
       </c>
       <c r="G18" s="11">
-        <v>6.0422222222222217</v>
+        <v>7.0422222222222217</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -1168,7 +1168,7 @@
         <v>4.7611111111111111</v>
       </c>
       <c r="G19" s="11">
-        <v>7.6111111111111107</v>
+        <v>8.6111111111111107</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -1200,7 +1200,7 @@
         <v>5.9136666666666677</v>
       </c>
       <c r="G20" s="11">
-        <v>9.706666666666667</v>
+        <v>10.706666666666667</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -1232,7 +1232,7 @@
         <v>5.4577777777777774</v>
       </c>
       <c r="G21" s="11">
-        <v>8.8777777777777782</v>
+        <v>9.8777777777777782</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -1296,7 +1296,7 @@
         <v>3.5229999999999997</v>
       </c>
       <c r="G23" s="11">
-        <v>5.3599999999999994</v>
+        <v>6.3599999999999994</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -1328,7 +1328,7 @@
         <v>4.5129999999999999</v>
       </c>
       <c r="G24" s="11">
-        <v>7.1599999999999993</v>
+        <v>8.16</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -1360,7 +1360,7 @@
         <v>6.0798888888888873</v>
       </c>
       <c r="G25" s="11">
-        <v>10.008888888888885</v>
+        <v>11.008888888888885</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>

</xml_diff>